<commit_message>
TS 1.3 Padam Input+TTD 06/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3999" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3991" uniqueCount="1303">
   <si>
     <t>PS</t>
   </si>
@@ -3653,12 +3653,6 @@
     <t>Vis</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>RE?</t>
-  </si>
-  <si>
     <t>aqyAsaq ityaqyAsa#H</t>
   </si>
   <si>
@@ -3716,9 +3710,6 @@
     <t>iqddha itIqddhaH ||</t>
   </si>
   <si>
-    <t>NE+re?</t>
-  </si>
-  <si>
     <t>aqntarityaqntaH</t>
   </si>
   <si>
@@ -3833,15 +3824,9 @@
     <t>NE+NSE</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>NE+NSE+NRE</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>yaqj~jiyA#saq iti# yaqj~jiyA#saH ||</t>
   </si>
   <si>
@@ -3911,9 +3896,6 @@
     <t>dyAvA#pRuthiqvI |</t>
   </si>
   <si>
-    <t>gm?</t>
-  </si>
-  <si>
     <t>suryaq iti# sUrya#H ||</t>
   </si>
   <si>
@@ -3942,19 +3924,37 @@
   </si>
   <si>
     <t>Sarddha$m |</t>
+  </si>
+  <si>
+    <t>n(H)</t>
+  </si>
+  <si>
+    <t>ceti# ca ||</t>
+  </si>
+  <si>
+    <t>NE+NRE</t>
+  </si>
+  <si>
+    <t>R( c)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4048,7 +4048,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4058,18 +4058,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4101,108 +4089,111 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4216,11 +4207,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4228,26 +4219,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4534,10 +4516,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="T97" sqref="T97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5442,7 +5424,7 @@
         <v>181</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
@@ -6025,7 +6007,7 @@
         <v>199</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
@@ -6514,7 +6496,7 @@
         <v>199</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
@@ -7356,7 +7338,7 @@
         <v>204</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P57" s="7"/>
       <c r="Q57" s="7"/>
@@ -7481,7 +7463,7 @@
         <v>181</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -8166,7 +8148,7 @@
         <v>1177</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P77" s="7"/>
       <c r="Q77" s="7"/>
@@ -8653,7 +8635,7 @@
         <v>181</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="P90" s="7"/>
       <c r="Q90" s="7"/>
@@ -8870,7 +8852,7 @@
         <v>1205</v>
       </c>
       <c r="T96" s="2" t="s">
-        <v>1180</v>
+        <v>1302</v>
       </c>
       <c r="X96" s="21"/>
     </row>
@@ -8901,7 +8883,7 @@
         <v>1177</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X97" s="21"/>
     </row>
@@ -9135,7 +9117,7 @@
         <v>136</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X105" s="21"/>
     </row>
@@ -9808,7 +9790,7 @@
         <v>204</v>
       </c>
       <c r="O128" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X128" s="21"/>
     </row>
@@ -11108,7 +11090,7 @@
         <v>182</v>
       </c>
       <c r="O172" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X172" s="21"/>
     </row>
@@ -11261,7 +11243,7 @@
         <v>198</v>
       </c>
       <c r="O177" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X177" s="21"/>
     </row>
@@ -11611,7 +11593,7 @@
         <v>198</v>
       </c>
       <c r="O189" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X189" s="21"/>
     </row>
@@ -11761,10 +11743,10 @@
         <v>75</v>
       </c>
       <c r="N194" s="12" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="O194" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X194" s="21"/>
     </row>
@@ -11917,7 +11899,7 @@
         <v>160</v>
       </c>
       <c r="O199" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X199" s="21"/>
     </row>
@@ -12075,7 +12057,7 @@
         <v>1177</v>
       </c>
       <c r="O204" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X204" s="21"/>
     </row>
@@ -12233,7 +12215,7 @@
         <v>1177</v>
       </c>
       <c r="O209" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X209" s="21"/>
     </row>
@@ -15367,7 +15349,7 @@
         <v>203</v>
       </c>
       <c r="O315" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X315" s="21"/>
     </row>
@@ -15482,6 +15464,12 @@
       <c r="N319" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="S319" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="T319" s="2" t="s">
+        <v>1299</v>
+      </c>
       <c r="X319" s="21"/>
     </row>
     <row r="320" spans="5:24" x14ac:dyDescent="0.25">
@@ -15513,14 +15501,8 @@
       <c r="P320" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="S320" s="2" t="s">
-        <v>1207</v>
-      </c>
-      <c r="T320" s="2" t="s">
-        <v>1208</v>
-      </c>
-      <c r="X320" s="49" t="s">
-        <v>1287</v>
+      <c r="X320" s="47" t="s">
+        <v>1282</v>
       </c>
     </row>
     <row r="321" spans="5:24" x14ac:dyDescent="0.25">
@@ -15709,7 +15691,7 @@
         <v>1180</v>
       </c>
       <c r="X326" s="42" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="327" spans="5:24" x14ac:dyDescent="0.25">
@@ -16149,7 +16131,7 @@
         <v>181</v>
       </c>
       <c r="O341" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X341" s="21"/>
     </row>
@@ -16291,8 +16273,11 @@
       <c r="N346" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="R346" s="44" t="s">
-        <v>1213</v>
+      <c r="S346" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="T346" s="2" t="s">
+        <v>1211</v>
       </c>
       <c r="X346" s="21"/>
     </row>
@@ -16633,7 +16618,7 @@
         <v>160</v>
       </c>
       <c r="O358" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X358" s="21"/>
     </row>
@@ -16897,7 +16882,7 @@
         <v>1207</v>
       </c>
       <c r="T367" s="2" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="X367" s="21"/>
     </row>
@@ -17136,7 +17121,7 @@
         <v>202</v>
       </c>
       <c r="O375" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X375" s="21"/>
     </row>
@@ -17222,14 +17207,11 @@
       <c r="N378" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="R378" s="44" t="s">
-        <v>1213</v>
-      </c>
       <c r="S378" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T378" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X378" s="21"/>
     </row>
@@ -17260,7 +17242,7 @@
         <v>72</v>
       </c>
       <c r="O379" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X379" s="21"/>
     </row>
@@ -17290,7 +17272,7 @@
         <v>203</v>
       </c>
       <c r="O380" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X380" s="21"/>
     </row>
@@ -18161,8 +18143,8 @@
       <c r="P410" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X410" s="45" t="s">
-        <v>1274</v>
+      <c r="X410" s="44" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="411" spans="4:24" x14ac:dyDescent="0.25">
@@ -18190,7 +18172,7 @@
         <v>1184</v>
       </c>
       <c r="O411" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X411" s="21"/>
     </row>
@@ -19124,8 +19106,8 @@
         <f t="shared" si="14"/>
         <v>34</v>
       </c>
-      <c r="N444" s="50" t="s">
-        <v>1288</v>
+      <c r="N444" s="45" t="s">
+        <v>1283</v>
       </c>
       <c r="X444" s="21"/>
     </row>
@@ -19298,7 +19280,7 @@
         <v>201</v>
       </c>
       <c r="O450" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X450" s="21"/>
     </row>
@@ -19418,7 +19400,7 @@
         <v>203</v>
       </c>
       <c r="O454" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X454" s="21"/>
     </row>
@@ -19510,7 +19492,7 @@
         <v>203</v>
       </c>
       <c r="O457" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X457" s="21"/>
     </row>
@@ -20613,7 +20595,7 @@
         <v>200</v>
       </c>
       <c r="O495" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X495" s="21"/>
     </row>
@@ -20992,7 +20974,7 @@
         <v>204</v>
       </c>
       <c r="O508" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X508" s="21"/>
     </row>
@@ -21079,7 +21061,7 @@
         <v>181</v>
       </c>
       <c r="O511" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X511" s="21"/>
     </row>
@@ -21334,11 +21316,8 @@
       <c r="N520" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="R520" s="44" t="s">
-        <v>1238</v>
-      </c>
       <c r="S520" s="2" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="X520" s="21"/>
     </row>
@@ -21488,7 +21467,7 @@
         <v>1180</v>
       </c>
       <c r="X525" s="39" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="526" spans="5:24" x14ac:dyDescent="0.25">
@@ -21720,7 +21699,7 @@
         <v>198</v>
       </c>
       <c r="O533" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X533" s="21"/>
     </row>
@@ -21782,7 +21761,7 @@
         <v>1180</v>
       </c>
       <c r="X535" s="42" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="536" spans="5:24" x14ac:dyDescent="0.25">
@@ -21957,7 +21936,7 @@
         <v>1180</v>
       </c>
       <c r="X541" s="12" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="542" spans="5:24" x14ac:dyDescent="0.25">
@@ -22046,7 +22025,7 @@
         <v>1180</v>
       </c>
       <c r="X544" s="42" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="545" spans="5:24" x14ac:dyDescent="0.25">
@@ -22247,7 +22226,7 @@
         <v>1180</v>
       </c>
       <c r="X551" s="39" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="552" spans="5:24" x14ac:dyDescent="0.25">
@@ -22558,7 +22537,7 @@
         <v>1177</v>
       </c>
       <c r="O561" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X561" s="21"/>
     </row>
@@ -22732,7 +22711,7 @@
         <v>0</v>
       </c>
       <c r="X567" s="42" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="568" spans="5:24" x14ac:dyDescent="0.25">
@@ -22936,7 +22915,7 @@
         <v>1177</v>
       </c>
       <c r="O574" s="2" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X574" s="21"/>
     </row>
@@ -23081,7 +23060,7 @@
         <v>1177</v>
       </c>
       <c r="O579" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X579" s="21"/>
     </row>
@@ -23337,7 +23316,7 @@
         <v>198</v>
       </c>
       <c r="O588" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X588" s="21"/>
     </row>
@@ -23371,8 +23350,8 @@
       <c r="P589" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X589" s="51" t="s">
-        <v>1289</v>
+      <c r="X589" s="48" t="s">
+        <v>1284</v>
       </c>
     </row>
     <row r="590" spans="5:24" x14ac:dyDescent="0.25">
@@ -23635,7 +23614,7 @@
         <v>182</v>
       </c>
       <c r="O598" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X598" s="21"/>
     </row>
@@ -23779,7 +23758,7 @@
         <v>496</v>
       </c>
       <c r="R603" s="2" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="X603" s="21"/>
     </row>
@@ -23951,14 +23930,11 @@
       <c r="N609" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="R609" s="2" t="s">
-        <v>1180</v>
-      </c>
       <c r="S609" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T609" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X609" s="21"/>
     </row>
@@ -24412,7 +24388,7 @@
         <v>205</v>
       </c>
       <c r="U625" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X625" s="36" t="s">
         <v>1186</v>
@@ -24557,13 +24533,13 @@
         <v>136</v>
       </c>
       <c r="O630" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="S630" s="2" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="T630" s="2" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="X630" s="21"/>
     </row>
@@ -24594,7 +24570,7 @@
         <v>182</v>
       </c>
       <c r="O631" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X631" s="21"/>
     </row>
@@ -24749,13 +24725,13 @@
         <v>136</v>
       </c>
       <c r="O636" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="S636" s="2" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="T636" s="2" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="X636" s="21"/>
     </row>
@@ -24786,7 +24762,7 @@
         <v>182</v>
       </c>
       <c r="O637" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X637" s="21"/>
     </row>
@@ -24971,8 +24947,8 @@
       <c r="P643" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X643" s="45" t="s">
-        <v>1275</v>
+      <c r="X643" s="44" t="s">
+        <v>1270</v>
       </c>
     </row>
     <row r="644" spans="5:24" x14ac:dyDescent="0.25">
@@ -25747,7 +25723,7 @@
         <v>1207</v>
       </c>
       <c r="T669" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X669" s="21"/>
     </row>
@@ -25812,7 +25788,7 @@
         <v>181</v>
       </c>
       <c r="O671" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X671" s="21"/>
     </row>
@@ -25988,7 +25964,7 @@
         <v>181</v>
       </c>
       <c r="O677" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X677" s="21"/>
     </row>
@@ -26047,8 +26023,8 @@
       <c r="N679" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="R679" s="44" t="s">
-        <v>1238</v>
+      <c r="S679" s="2" t="s">
+        <v>1235</v>
       </c>
       <c r="X679" s="21"/>
     </row>
@@ -26201,7 +26177,7 @@
         <v>182</v>
       </c>
       <c r="O684" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X684" s="21"/>
     </row>
@@ -26574,7 +26550,7 @@
         <v>201</v>
       </c>
       <c r="O697" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X697" s="21"/>
     </row>
@@ -26722,7 +26698,7 @@
         <v>201</v>
       </c>
       <c r="O702" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X702" s="21"/>
     </row>
@@ -26809,7 +26785,7 @@
         <v>201</v>
       </c>
       <c r="O705" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X705" s="21"/>
     </row>
@@ -27051,7 +27027,7 @@
         <v>0</v>
       </c>
       <c r="R713" s="2" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="X713" s="21" t="s">
         <v>84</v>
@@ -27087,7 +27063,7 @@
         <v>0</v>
       </c>
       <c r="Q714" s="2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="X714" s="21" t="s">
         <v>558</v>
@@ -27120,7 +27096,7 @@
         <v>181</v>
       </c>
       <c r="O715" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X715" s="21"/>
     </row>
@@ -27444,7 +27420,7 @@
         <v>201</v>
       </c>
       <c r="O726" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X726" s="21"/>
     </row>
@@ -27882,7 +27858,10 @@
         <v>574</v>
       </c>
       <c r="S741" s="2" t="s">
-        <v>1265</v>
+        <v>1262</v>
+      </c>
+      <c r="T741" s="2" t="s">
+        <v>1261</v>
       </c>
       <c r="X741" s="21"/>
     </row>
@@ -27913,7 +27892,7 @@
         <v>182</v>
       </c>
       <c r="O742" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X742" s="21"/>
     </row>
@@ -28028,7 +28007,7 @@
         <v>136</v>
       </c>
       <c r="O746" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X746" s="21"/>
     </row>
@@ -28150,6 +28129,9 @@
       <c r="S750" s="2" t="s">
         <v>1207</v>
       </c>
+      <c r="T750" s="2" t="s">
+        <v>1257</v>
+      </c>
       <c r="X750" s="21"/>
     </row>
     <row r="751" spans="5:24" x14ac:dyDescent="0.25">
@@ -28259,14 +28241,14 @@
         <f t="shared" si="24"/>
         <v>84</v>
       </c>
-      <c r="N754" s="46" t="s">
-        <v>1276</v>
+      <c r="N754" s="45" t="s">
+        <v>1271</v>
       </c>
       <c r="O754" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="X754" s="45" t="s">
-        <v>1277</v>
+      <c r="X754" s="44" t="s">
+        <v>1272</v>
       </c>
     </row>
     <row r="755" spans="5:24" x14ac:dyDescent="0.25">
@@ -28352,10 +28334,10 @@
         <v>94</v>
       </c>
       <c r="S757" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="V757" s="2" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="X757" s="21"/>
     </row>
@@ -28566,8 +28548,8 @@
       <c r="P764" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X764" s="51" t="s">
-        <v>1290</v>
+      <c r="X764" s="48" t="s">
+        <v>1285</v>
       </c>
     </row>
     <row r="765" spans="5:24" x14ac:dyDescent="0.25">
@@ -28652,7 +28634,7 @@
         <v>181</v>
       </c>
       <c r="O767" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X767" s="21"/>
     </row>
@@ -28772,7 +28754,7 @@
         <v>181</v>
       </c>
       <c r="O771" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X771" s="21"/>
     </row>
@@ -28887,7 +28869,7 @@
         <v>181</v>
       </c>
       <c r="O775" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X775" s="21"/>
     </row>
@@ -29002,7 +28984,7 @@
         <v>181</v>
       </c>
       <c r="O779" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X779" s="21"/>
     </row>
@@ -29122,10 +29104,10 @@
         <v>0</v>
       </c>
       <c r="S783" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="V783" s="2" t="s">
-        <v>1278</v>
+        <v>1273</v>
       </c>
       <c r="X783" s="21" t="s">
         <v>584</v>
@@ -29532,7 +29514,7 @@
         <v>181</v>
       </c>
       <c r="O797" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X797" s="21"/>
     </row>
@@ -29760,7 +29742,7 @@
         <v>181</v>
       </c>
       <c r="O805" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X805" s="21"/>
     </row>
@@ -29875,7 +29857,7 @@
         <v>181</v>
       </c>
       <c r="O809" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X809" s="21"/>
     </row>
@@ -30081,8 +30063,8 @@
       <c r="O816" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="X816" s="45" t="s">
-        <v>1279</v>
+      <c r="X816" s="44" t="s">
+        <v>1274</v>
       </c>
     </row>
     <row r="817" spans="5:24" x14ac:dyDescent="0.25">
@@ -31142,7 +31124,7 @@
         <v>182</v>
       </c>
       <c r="O853" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X853" s="21"/>
     </row>
@@ -31346,7 +31328,7 @@
         <v>136</v>
       </c>
       <c r="O860" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X860" s="21"/>
     </row>
@@ -31439,7 +31421,7 @@
         <v>203</v>
       </c>
       <c r="O863" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X863" s="21"/>
     </row>
@@ -31617,8 +31599,8 @@
       <c r="P869" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X869" s="51" t="s">
-        <v>1291</v>
+      <c r="X869" s="48" t="s">
+        <v>1286</v>
       </c>
     </row>
     <row r="870" spans="5:24" x14ac:dyDescent="0.25">
@@ -31646,7 +31628,7 @@
         <v>201</v>
       </c>
       <c r="O870" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X870" s="21"/>
     </row>
@@ -31762,7 +31744,7 @@
         <v>201</v>
       </c>
       <c r="O874" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X874" s="21"/>
     </row>
@@ -32067,8 +32049,8 @@
       <c r="O884" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T884" s="2" t="s">
-        <v>1267</v>
+      <c r="U884" s="2" t="s">
+        <v>1264</v>
       </c>
       <c r="X884" s="21" t="s">
         <v>609</v>
@@ -32101,7 +32083,7 @@
         <v>1175</v>
       </c>
       <c r="O885" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X885" s="21"/>
     </row>
@@ -32224,7 +32206,7 @@
         <v>0</v>
       </c>
       <c r="U889" s="2" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="X889" s="21" t="s">
         <v>609</v>
@@ -32257,7 +32239,7 @@
         <v>203</v>
       </c>
       <c r="O890" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X890" s="21"/>
     </row>
@@ -32343,14 +32325,11 @@
       <c r="N893" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="R893" s="2" t="s">
-        <v>1180</v>
-      </c>
       <c r="S893" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T893" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X893" s="21"/>
     </row>
@@ -32738,7 +32717,7 @@
         <v>136</v>
       </c>
       <c r="O906" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X906" s="21"/>
     </row>
@@ -32822,7 +32801,7 @@
         <v>40</v>
       </c>
       <c r="N909" s="12" t="s">
-        <v>1292</v>
+        <v>1287</v>
       </c>
       <c r="O909" s="15"/>
       <c r="X909" s="21"/>
@@ -32938,9 +32917,6 @@
       <c r="N913" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="U913" s="44" t="s">
-        <v>1209</v>
-      </c>
       <c r="X913" s="21"/>
     </row>
     <row r="914" spans="5:24" x14ac:dyDescent="0.25">
@@ -33054,7 +33030,7 @@
         <v>201</v>
       </c>
       <c r="O917" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X917" s="21"/>
     </row>
@@ -34254,7 +34230,7 @@
         <v>1183</v>
       </c>
       <c r="U958" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X958" s="21" t="s">
         <v>646</v>
@@ -34682,7 +34658,7 @@
         <v>26</v>
       </c>
       <c r="N973" s="12" t="s">
-        <v>1293</v>
+        <v>1288</v>
       </c>
       <c r="O973" s="2" t="s">
         <v>1183</v>
@@ -35432,7 +35408,7 @@
         <v>1176</v>
       </c>
       <c r="O999" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X999" s="21"/>
     </row>
@@ -36124,7 +36100,7 @@
         <v>1180</v>
       </c>
       <c r="X1023" s="40" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1024" spans="5:24" x14ac:dyDescent="0.25">
@@ -36207,9 +36183,6 @@
       <c r="N1026" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="R1026" s="2" t="s">
-        <v>1294</v>
-      </c>
       <c r="X1026" s="21"/>
     </row>
     <row r="1027" spans="5:24" x14ac:dyDescent="0.25">
@@ -36295,7 +36268,7 @@
         <v>156</v>
       </c>
       <c r="U1029" s="2" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="X1029" s="21"/>
     </row>
@@ -36326,10 +36299,10 @@
         <v>669</v>
       </c>
       <c r="S1030" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="V1030" s="2" t="s">
-        <v>1280</v>
+        <v>1275</v>
       </c>
       <c r="X1030" s="21"/>
     </row>
@@ -36360,7 +36333,7 @@
         <v>181</v>
       </c>
       <c r="O1031" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1031" s="21"/>
     </row>
@@ -36421,10 +36394,10 @@
       </c>
       <c r="O1033" s="2"/>
       <c r="S1033" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="V1033" s="2" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="X1033" s="21"/>
     </row>
@@ -36454,6 +36427,9 @@
       <c r="N1034" s="12" t="s">
         <v>671</v>
       </c>
+      <c r="U1034" s="2" t="s">
+        <v>1267</v>
+      </c>
       <c r="X1034" s="21"/>
     </row>
     <row r="1035" spans="5:24" x14ac:dyDescent="0.25">
@@ -36485,8 +36461,8 @@
       <c r="P1035" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1035" s="51" t="s">
-        <v>1295</v>
+      <c r="X1035" s="48" t="s">
+        <v>1289</v>
       </c>
     </row>
     <row r="1036" spans="5:24" x14ac:dyDescent="0.25">
@@ -36516,9 +36492,6 @@
         <v>88</v>
       </c>
       <c r="O1036" s="2"/>
-      <c r="U1036" s="2" t="s">
-        <v>1268</v>
-      </c>
       <c r="X1036" s="21"/>
     </row>
     <row r="1037" spans="5:24" x14ac:dyDescent="0.25">
@@ -37142,7 +37115,7 @@
         <v>1180</v>
       </c>
       <c r="X1057" s="40" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1058" spans="5:24" x14ac:dyDescent="0.25">
@@ -37677,7 +37650,7 @@
         <v>181</v>
       </c>
       <c r="O1076" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1076" s="21"/>
     </row>
@@ -37736,7 +37709,7 @@
         <v>198</v>
       </c>
       <c r="O1078" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1078" s="21"/>
     </row>
@@ -37879,7 +37852,7 @@
         <v>201</v>
       </c>
       <c r="O1083" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1083" s="21"/>
     </row>
@@ -38473,7 +38446,7 @@
         <v>1180</v>
       </c>
       <c r="X1103" s="40" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1104" spans="5:24" x14ac:dyDescent="0.25">
@@ -38758,7 +38731,7 @@
         <v>1180</v>
       </c>
       <c r="X1113" s="40" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1114" spans="5:24" x14ac:dyDescent="0.25">
@@ -39399,7 +39372,7 @@
         <v>197</v>
       </c>
       <c r="O1135" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1135" s="21"/>
     </row>
@@ -39571,7 +39544,7 @@
         <v>204</v>
       </c>
       <c r="O1141" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1141" s="21"/>
     </row>
@@ -39604,8 +39577,8 @@
       <c r="P1142" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1142" s="48" t="s">
-        <v>1281</v>
+      <c r="X1142" s="46" t="s">
+        <v>1276</v>
       </c>
     </row>
     <row r="1143" spans="5:24" x14ac:dyDescent="0.25">
@@ -39751,8 +39724,6 @@
       <c r="N1147" s="12" t="s">
         <v>720</v>
       </c>
-      <c r="S1147" s="47"/>
-      <c r="T1147" s="47"/>
       <c r="X1147" s="21"/>
     </row>
     <row r="1148" spans="5:24" x14ac:dyDescent="0.25">
@@ -39843,7 +39814,7 @@
         <v>1180</v>
       </c>
       <c r="X1150" s="12" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1151" spans="5:24" x14ac:dyDescent="0.25">
@@ -39959,8 +39930,8 @@
       <c r="P1154" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1154" s="51" t="s">
-        <v>1296</v>
+      <c r="X1154" s="48" t="s">
+        <v>1290</v>
       </c>
     </row>
     <row r="1155" spans="5:24" x14ac:dyDescent="0.25">
@@ -40017,7 +39988,7 @@
       </c>
       <c r="O1156" s="2"/>
       <c r="U1156" s="2" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="X1156" s="21"/>
     </row>
@@ -40076,7 +40047,7 @@
         <v>727</v>
       </c>
       <c r="U1158" s="2" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="X1158" s="21"/>
     </row>
@@ -40280,7 +40251,7 @@
         <v>1180</v>
       </c>
       <c r="X1165" s="12" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1166" spans="5:24" x14ac:dyDescent="0.25">
@@ -40604,7 +40575,7 @@
         <v>1180</v>
       </c>
       <c r="X1176" s="41" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1177" spans="5:24" x14ac:dyDescent="0.25">
@@ -40634,7 +40605,7 @@
         <v>181</v>
       </c>
       <c r="O1177" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1177" s="21"/>
     </row>
@@ -40840,8 +40811,8 @@
       <c r="P1184" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1184" s="51" t="s">
-        <v>1297</v>
+      <c r="X1184" s="48" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row r="1185" spans="5:24" x14ac:dyDescent="0.25">
@@ -41047,7 +41018,7 @@
         <v>1180</v>
       </c>
       <c r="X1191" s="40" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1192" spans="5:24" x14ac:dyDescent="0.25">
@@ -41133,7 +41104,7 @@
         <v>1175</v>
       </c>
       <c r="O1194" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1194" s="21"/>
     </row>
@@ -41163,8 +41134,8 @@
       <c r="N1195" s="12" t="s">
         <v>749</v>
       </c>
-      <c r="R1195" s="44" t="s">
-        <v>1298</v>
+      <c r="S1195" s="2" t="s">
+        <v>1292</v>
       </c>
       <c r="X1195" s="21"/>
     </row>
@@ -41343,7 +41314,7 @@
         <v>1180</v>
       </c>
       <c r="X1201" s="40" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1202" spans="5:24" x14ac:dyDescent="0.25">
@@ -41464,7 +41435,7 @@
       <c r="O1205" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="X1205" s="45" t="s">
+      <c r="X1205" s="44" t="s">
         <v>756</v>
       </c>
     </row>
@@ -41611,7 +41582,7 @@
         <v>1180</v>
       </c>
       <c r="X1210" s="12" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1211" spans="5:24" x14ac:dyDescent="0.25">
@@ -41668,14 +41639,11 @@
       <c r="N1212" s="12" t="s">
         <v>762</v>
       </c>
-      <c r="R1212" s="2" t="s">
-        <v>1213</v>
-      </c>
       <c r="S1212" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T1212" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1212" s="21"/>
     </row>
@@ -41887,7 +41855,7 @@
         <v>1180</v>
       </c>
       <c r="X1219" s="12" t="s">
-        <v>1282</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1220" spans="5:24" x14ac:dyDescent="0.25">
@@ -41974,7 +41942,7 @@
         <v>181</v>
       </c>
       <c r="O1222" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1222" s="21"/>
     </row>
@@ -42116,14 +42084,11 @@
       <c r="N1227" s="12" t="s">
         <v>762</v>
       </c>
-      <c r="R1227" s="2" t="s">
-        <v>1213</v>
-      </c>
       <c r="S1227" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T1227" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1227" s="21"/>
     </row>
@@ -42220,8 +42185,8 @@
       <c r="U1230" s="2" t="s">
         <v>1206</v>
       </c>
-      <c r="X1230" s="45" t="s">
-        <v>1283</v>
+      <c r="X1230" s="44" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="1231" spans="5:24" x14ac:dyDescent="0.25">
@@ -42391,8 +42356,8 @@
       <c r="N1236" s="12" t="s">
         <v>774</v>
       </c>
-      <c r="R1236" s="44" t="s">
-        <v>1238</v>
+      <c r="S1236" s="2" t="s">
+        <v>1235</v>
       </c>
       <c r="X1236" s="21"/>
     </row>
@@ -42571,7 +42536,7 @@
         <v>203</v>
       </c>
       <c r="O1242" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1242" s="21"/>
     </row>
@@ -42659,9 +42624,6 @@
       <c r="N1245" s="12" t="s">
         <v>780</v>
       </c>
-      <c r="S1245" s="2" t="s">
-        <v>1270</v>
-      </c>
       <c r="X1245" s="21"/>
     </row>
     <row r="1246" spans="5:24" x14ac:dyDescent="0.25">
@@ -42691,7 +42653,7 @@
         <v>781</v>
       </c>
       <c r="U1246" s="2" t="s">
-        <v>1229</v>
+        <v>1301</v>
       </c>
       <c r="X1246" s="21"/>
     </row>
@@ -42722,7 +42684,7 @@
         <v>181</v>
       </c>
       <c r="O1247" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1247" s="21"/>
     </row>
@@ -42844,17 +42806,14 @@
       <c r="P1251" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="R1251" s="2" t="s">
-        <v>1213</v>
-      </c>
       <c r="S1251" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T1251" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1251" s="40" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1252" spans="5:24" x14ac:dyDescent="0.25">
@@ -42881,13 +42840,13 @@
         <v>98</v>
       </c>
       <c r="N1252" s="12" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="O1252" s="2" t="s">
         <v>205</v>
       </c>
       <c r="X1252" s="40" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1253" spans="5:24" x14ac:dyDescent="0.25">
@@ -42976,14 +42935,11 @@
       <c r="N1255" s="12" t="s">
         <v>785</v>
       </c>
-      <c r="R1255" s="2" t="s">
-        <v>1213</v>
-      </c>
       <c r="S1255" s="2" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="T1255" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1255" s="21"/>
     </row>
@@ -43042,10 +42998,10 @@
         <v>787</v>
       </c>
       <c r="S1257" s="2" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="T1257" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1257" s="21"/>
     </row>
@@ -43076,7 +43032,7 @@
         <v>181</v>
       </c>
       <c r="O1258" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1258" s="21"/>
     </row>
@@ -43138,7 +43094,7 @@
         <v>1180</v>
       </c>
       <c r="X1260" s="43" t="s">
-        <v>1271</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1261" spans="5:24" x14ac:dyDescent="0.25">
@@ -43308,7 +43264,7 @@
         <v>201</v>
       </c>
       <c r="O1266" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1266" s="21"/>
     </row>
@@ -43398,7 +43354,7 @@
         <v>1180</v>
       </c>
       <c r="X1269" s="40" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1270" spans="5:24" x14ac:dyDescent="0.25">
@@ -43582,8 +43538,8 @@
       <c r="P1275" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1275" s="51" t="s">
-        <v>1299</v>
+      <c r="X1275" s="48" t="s">
+        <v>1293</v>
       </c>
     </row>
     <row r="1276" spans="5:24" x14ac:dyDescent="0.25">
@@ -43673,7 +43629,7 @@
         <v>1180</v>
       </c>
       <c r="X1278" s="40" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1279" spans="5:24" x14ac:dyDescent="0.25">
@@ -43789,7 +43745,7 @@
         <v>97</v>
       </c>
       <c r="U1282" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X1282" s="21"/>
     </row>
@@ -44058,7 +44014,7 @@
         <v>1176</v>
       </c>
       <c r="O1291" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1291" s="21"/>
     </row>
@@ -44202,7 +44158,7 @@
         <v>811</v>
       </c>
       <c r="U1296" s="2" t="s">
-        <v>1272</v>
+        <v>1267</v>
       </c>
       <c r="X1296" s="21"/>
     </row>
@@ -44411,7 +44367,7 @@
         <v>181</v>
       </c>
       <c r="O1303" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1303" s="21"/>
     </row>
@@ -44444,8 +44400,8 @@
       <c r="P1304" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1304" s="51" t="s">
-        <v>1300</v>
+      <c r="X1304" s="48" t="s">
+        <v>1294</v>
       </c>
     </row>
     <row r="1305" spans="5:24" x14ac:dyDescent="0.25">
@@ -44542,8 +44498,8 @@
       <c r="P1307" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1307" s="51" t="s">
-        <v>1301</v>
+      <c r="X1307" s="48" t="s">
+        <v>1295</v>
       </c>
     </row>
     <row r="1308" spans="5:24" x14ac:dyDescent="0.25">
@@ -44993,7 +44949,7 @@
         <v>1180</v>
       </c>
       <c r="X1322" s="43" t="s">
-        <v>1273</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1323" spans="5:24" x14ac:dyDescent="0.25">
@@ -45189,13 +45145,13 @@
         <v>175</v>
       </c>
       <c r="N1329" s="12" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="P1329" s="2" t="s">
         <v>1180</v>
       </c>
       <c r="X1329" s="40" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1330" spans="5:24" x14ac:dyDescent="0.25">
@@ -45315,7 +45271,7 @@
         <v>181</v>
       </c>
       <c r="O1333" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1333" s="21"/>
     </row>
@@ -45374,10 +45330,10 @@
         <v>1174</v>
       </c>
       <c r="O1335" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="S1335" s="2" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="X1335" s="21"/>
     </row>
@@ -45532,7 +45488,7 @@
         <v>97</v>
       </c>
       <c r="U1340" s="2" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="X1340" s="21"/>
     </row>
@@ -45688,7 +45644,7 @@
         <v>1180</v>
       </c>
       <c r="X1345" s="40" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1346" spans="5:24" x14ac:dyDescent="0.25">
@@ -45943,7 +45899,7 @@
         <v>1176</v>
       </c>
       <c r="O1354" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1354" s="21"/>
     </row>
@@ -46004,8 +45960,8 @@
       <c r="P1356" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1356" s="51" t="s">
-        <v>1302</v>
+      <c r="X1356" s="48" t="s">
+        <v>1296</v>
       </c>
     </row>
     <row r="1357" spans="5:24" x14ac:dyDescent="0.25">
@@ -46286,8 +46242,11 @@
       <c r="N1365" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="R1365" s="2" t="s">
-        <v>1260</v>
+      <c r="S1365" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="T1365" s="2" t="s">
+        <v>1257</v>
       </c>
       <c r="X1365" s="21"/>
     </row>
@@ -46318,7 +46277,7 @@
         <v>1177</v>
       </c>
       <c r="O1366" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1366" s="21"/>
     </row>
@@ -46492,7 +46451,7 @@
         <v>1177</v>
       </c>
       <c r="O1372" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1372" s="21"/>
     </row>
@@ -46942,7 +46901,7 @@
         <v>203</v>
       </c>
       <c r="O1387" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1387" s="21"/>
     </row>
@@ -46976,7 +46935,7 @@
         <v>1180</v>
       </c>
       <c r="X1388" s="40" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1389" spans="5:24" x14ac:dyDescent="0.25">
@@ -47184,7 +47143,7 @@
         <v>203</v>
       </c>
       <c r="O1395" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1395" s="21"/>
     </row>
@@ -47335,7 +47294,7 @@
         <v>1180</v>
       </c>
       <c r="X1400" s="40" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1401" spans="5:24" x14ac:dyDescent="0.25">
@@ -47364,8 +47323,8 @@
       <c r="N1401" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="U1401" s="44" t="s">
-        <v>1272</v>
+      <c r="U1401" s="2" t="s">
+        <v>1267</v>
       </c>
       <c r="X1401" s="21"/>
     </row>
@@ -47396,7 +47355,7 @@
         <v>877</v>
       </c>
       <c r="U1402" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X1402" s="21"/>
     </row>
@@ -47641,7 +47600,7 @@
         <v>181</v>
       </c>
       <c r="O1410" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1410" s="21"/>
     </row>
@@ -47937,10 +47896,10 @@
         <v>1180</v>
       </c>
       <c r="U1420" s="2" t="s">
-        <v>1225</v>
-      </c>
-      <c r="X1420" s="51" t="s">
-        <v>1303</v>
+        <v>1223</v>
+      </c>
+      <c r="X1420" s="48" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="1421" spans="5:24" x14ac:dyDescent="0.25">
@@ -47995,7 +47954,7 @@
         <v>268</v>
       </c>
       <c r="N1422" s="12" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="X1422" s="21"/>
     </row>
@@ -48175,7 +48134,7 @@
         <v>1180</v>
       </c>
       <c r="X1428" s="40" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1429" spans="5:24" x14ac:dyDescent="0.25">
@@ -48413,7 +48372,7 @@
         <v>1180</v>
       </c>
       <c r="X1436" s="40" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1437" spans="5:24" x14ac:dyDescent="0.25">
@@ -48684,8 +48643,8 @@
       <c r="P1445" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1445" s="45" t="s">
-        <v>1284</v>
+      <c r="X1445" s="44" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="1446" spans="5:24" x14ac:dyDescent="0.25">
@@ -48771,7 +48730,7 @@
         <v>181</v>
       </c>
       <c r="O1448" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1448" s="21"/>
     </row>
@@ -48894,7 +48853,7 @@
         <v>1180</v>
       </c>
       <c r="X1452" s="40" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1453" spans="5:24" x14ac:dyDescent="0.25">
@@ -49005,10 +48964,10 @@
         <v>302</v>
       </c>
       <c r="N1456" s="12" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="O1456" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1456" s="21"/>
     </row>
@@ -49101,7 +49060,7 @@
         <v>1180</v>
       </c>
       <c r="X1459" s="40" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1460" spans="5:24" x14ac:dyDescent="0.25">
@@ -49159,7 +49118,7 @@
         <v>97</v>
       </c>
       <c r="U1461" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X1461" s="21"/>
     </row>
@@ -49279,7 +49238,7 @@
         <v>181</v>
       </c>
       <c r="O1465" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1465" s="21"/>
     </row>
@@ -49312,8 +49271,8 @@
       <c r="P1466" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1466" s="51" t="s">
-        <v>1300</v>
+      <c r="X1466" s="48" t="s">
+        <v>1294</v>
       </c>
     </row>
     <row r="1467" spans="5:24" x14ac:dyDescent="0.25">
@@ -49427,7 +49386,7 @@
         <v>914</v>
       </c>
       <c r="U1470" s="2" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="X1470" s="21"/>
     </row>
@@ -49652,7 +49611,7 @@
         <v>1180</v>
       </c>
       <c r="X1477" s="12" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1478" spans="5:24" x14ac:dyDescent="0.25">
@@ -49741,10 +49700,10 @@
         <v>1180</v>
       </c>
       <c r="U1480" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="X1480" s="40" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1481" spans="5:24" x14ac:dyDescent="0.25">
@@ -50047,7 +50006,7 @@
         <v>1180</v>
       </c>
       <c r="X1490" s="40" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1491" spans="5:24" x14ac:dyDescent="0.25">
@@ -50392,17 +50351,14 @@
       <c r="P1502" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="R1502" s="2" t="s">
-        <v>1213</v>
-      </c>
       <c r="S1502" s="2" t="s">
         <v>1207</v>
       </c>
       <c r="T1502" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X1502" s="40" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1503" spans="5:24" x14ac:dyDescent="0.25">
@@ -50516,7 +50472,7 @@
         <v>181</v>
       </c>
       <c r="O1506" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1506" s="21"/>
     </row>
@@ -50661,7 +50617,7 @@
       <c r="P1511" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1511" s="51" t="s">
+      <c r="X1511" s="48" t="s">
         <v>1187</v>
       </c>
     </row>
@@ -50751,7 +50707,7 @@
         <v>1180</v>
       </c>
       <c r="X1514" s="40" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1515" spans="5:24" x14ac:dyDescent="0.25">
@@ -50873,7 +50829,7 @@
         <v>205</v>
       </c>
       <c r="U1518" s="2" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="X1518" s="38" t="s">
         <v>1204</v>
@@ -51058,7 +51014,7 @@
         <v>1180</v>
       </c>
       <c r="X1524" s="40" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1525" spans="5:24" x14ac:dyDescent="0.25">
@@ -51232,7 +51188,7 @@
         <v>1180</v>
       </c>
       <c r="X1530" s="40" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1531" spans="5:24" x14ac:dyDescent="0.25">
@@ -51262,7 +51218,7 @@
         <v>181</v>
       </c>
       <c r="O1531" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1531" s="21"/>
     </row>
@@ -51379,8 +51335,8 @@
       <c r="P1535" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1535" s="40" t="s">
-        <v>1242</v>
+      <c r="X1535" s="49" t="s">
+        <v>1300</v>
       </c>
     </row>
     <row r="1536" spans="5:24" x14ac:dyDescent="0.25">
@@ -51550,10 +51506,10 @@
         <v>94</v>
       </c>
       <c r="S1541" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="V1541" s="2" t="s">
-        <v>1285</v>
+        <v>1280</v>
       </c>
       <c r="X1541" s="21"/>
     </row>
@@ -51612,7 +51568,7 @@
         <v>181</v>
       </c>
       <c r="O1543" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1543" s="21"/>
     </row>
@@ -51646,7 +51602,7 @@
         <v>1180</v>
       </c>
       <c r="X1544" s="40" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1545" spans="5:24" x14ac:dyDescent="0.25">
@@ -51790,7 +51746,7 @@
       <c r="P1549" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="X1549" s="51" t="s">
+      <c r="X1549" s="48" t="s">
         <v>1187</v>
       </c>
     </row>
@@ -51969,7 +51925,7 @@
         <v>1180</v>
       </c>
       <c r="X1555" s="12" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1556" spans="5:24" x14ac:dyDescent="0.25">
@@ -52091,7 +52047,7 @@
         <v>204</v>
       </c>
       <c r="O1559" s="1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="X1559" s="21"/>
     </row>
@@ -52122,7 +52078,7 @@
         <v>97</v>
       </c>
       <c r="U1560" s="2" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="X1560" s="21"/>
     </row>
@@ -52271,7 +52227,7 @@
         <v>1180</v>
       </c>
       <c r="X1565" s="40" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1566" spans="5:24" x14ac:dyDescent="0.25">
@@ -52360,10 +52316,10 @@
         <v>1180</v>
       </c>
       <c r="U1568" s="2" t="s">
-        <v>1225</v>
-      </c>
-      <c r="X1568" s="45" t="s">
-        <v>1286</v>
+        <v>1223</v>
+      </c>
+      <c r="X1568" s="44" t="s">
+        <v>1281</v>
       </c>
     </row>
     <row r="1569" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edits to Padam Excel and Rule files/TTD
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
@@ -4570,10 +4570,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1557" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1136" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="U1550" sqref="U1550"/>
+      <selection pane="bottomLeft" activeCell="X1145" sqref="X1145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Padam changes Kramam corr 20/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.3 Padam Input Template.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4031,7 +4031,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4703,10 +4703,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1327" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1318" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="L1330" sqref="L1330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>